<commit_message>
fixed mistakes in the xkls file
</commit_message>
<xml_diff>
--- a/Fwd__bowling_ver10/rawData/data/before_Sheet_firstRound.xlsx
+++ b/Fwd__bowling_ver10/rawData/data/before_Sheet_firstRound.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download_from_chrome\Fwd__bowling_ver11\Fwd__bowling_ver10\rawData\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="16020" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -21,12 +26,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="3">גיליון4!$A:$K,גיליון4!$1:$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">גיליון5!$A:$K,גיליון5!$1:$47</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="61">
   <si>
     <t>אגודת כדורת - אשדוד</t>
   </si>
@@ -181,13 +186,43 @@
   </si>
   <si>
     <t>חתימת קפטן קבוצה 3:</t>
+  </si>
+  <si>
+    <t>קבוצה 6</t>
+  </si>
+  <si>
+    <t>קבוצה 7</t>
+  </si>
+  <si>
+    <t>קבוצה 8</t>
+  </si>
+  <si>
+    <t>קבוצה 9</t>
+  </si>
+  <si>
+    <t>קבוצה 10</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 6:</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 8:</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 7:</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 9:</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 10:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +471,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -482,7 +525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -514,9 +557,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,6 +609,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -723,20 +802,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
@@ -744,13 +823,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -768,7 +847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -786,7 +865,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -804,7 +883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -822,7 +901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -839,7 +918,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -847,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
         <v>43</v>
       </c>
@@ -859,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
@@ -868,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
@@ -877,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -888,7 +967,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -915,7 +994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>0</v>
       </c>
@@ -932,7 +1011,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -949,7 +1028,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>0</v>
       </c>
@@ -966,7 +1045,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
@@ -984,7 +1063,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
@@ -1018,7 +1097,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
@@ -1029,7 +1108,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>42</v>
       </c>
@@ -1040,7 +1119,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1053,8 +1132,8 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="15" thickTop="1"/>
-    <row r="27" spans="1:11" ht="18">
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
         <v>41</v>
       </c>
@@ -1066,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1095,7 +1174,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
@@ -1122,7 +1201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>0</v>
       </c>
@@ -1139,7 +1218,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>0</v>
       </c>
@@ -1156,7 +1235,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>0</v>
       </c>
@@ -1173,7 +1252,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
@@ -1191,7 +1270,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
@@ -1214,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
@@ -1225,7 +1304,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1315,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>44</v>
       </c>
@@ -1247,7 +1326,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1260,8 +1339,8 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickTop="1"/>
-    <row r="44" spans="1:11" ht="23.25">
+    <row r="43" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>40</v>
       </c>
@@ -1318,20 +1397,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1339,13 +1418,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -1381,7 +1460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1399,7 +1478,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -1417,7 +1496,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1434,7 +1513,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1442,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
         <v>49</v>
       </c>
@@ -1454,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1463,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1472,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1483,7 +1562,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -1510,7 +1589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>0</v>
       </c>
@@ -1527,7 +1606,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -1544,7 +1623,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>0</v>
       </c>
@@ -1561,7 +1640,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
@@ -1579,7 +1658,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1692,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
@@ -1624,7 +1703,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>26</v>
       </c>
@@ -1635,7 +1714,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1648,8 +1727,8 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="15" thickTop="1"/>
-    <row r="27" spans="1:11" ht="18">
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
@@ -1670,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1690,7 +1769,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
@@ -1717,7 +1796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>0</v>
       </c>
@@ -1734,7 +1813,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>0</v>
       </c>
@@ -1751,7 +1830,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>0</v>
       </c>
@@ -1768,7 +1847,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
@@ -1786,7 +1865,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
@@ -1809,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
@@ -1820,7 +1899,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +1910,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>50</v>
       </c>
@@ -1842,7 +1921,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1855,8 +1934,8 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickTop="1"/>
-    <row r="44" spans="1:11" ht="23.25">
+    <row r="43" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>40</v>
       </c>
@@ -1913,20 +1992,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView rightToLeft="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1934,13 +2013,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +2037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -1976,7 +2055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1994,7 +2073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -2012,7 +2091,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2029,7 +2108,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2037,9 +2116,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>12</v>
@@ -2049,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
@@ -2058,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
@@ -2067,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2078,7 +2157,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -2105,7 +2184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>0</v>
       </c>
@@ -2122,7 +2201,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -2139,7 +2218,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>0</v>
       </c>
@@ -2156,7 +2235,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
@@ -2174,7 +2253,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
@@ -2197,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
@@ -2208,7 +2287,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
@@ -2219,9 +2298,9 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="26"/>
@@ -2230,7 +2309,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2243,10 +2322,10 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="15" thickTop="1"/>
-    <row r="27" spans="1:11" ht="18">
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>12</v>
@@ -2256,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
@@ -2265,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
@@ -2274,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2285,7 +2364,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
@@ -2312,7 +2391,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>0</v>
       </c>
@@ -2329,7 +2408,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>0</v>
       </c>
@@ -2346,7 +2425,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>0</v>
       </c>
@@ -2363,7 +2442,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
@@ -2381,7 +2460,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
@@ -2415,7 +2494,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
@@ -2426,9 +2505,9 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="26"/>
@@ -2437,7 +2516,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2450,8 +2529,8 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickTop="1"/>
-    <row r="44" spans="1:11" ht="23.25">
+    <row r="43" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>40</v>
       </c>
@@ -2508,20 +2587,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView rightToLeft="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2529,13 +2608,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -2553,7 +2632,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -2571,7 +2650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -2589,7 +2668,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -2607,7 +2686,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2624,7 +2703,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2632,9 +2711,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>12</v>
@@ -2644,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
@@ -2653,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
@@ -2662,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2673,7 +2752,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -2700,7 +2779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>0</v>
       </c>
@@ -2717,7 +2796,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -2734,7 +2813,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>0</v>
       </c>
@@ -2751,7 +2830,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
@@ -2769,7 +2848,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
@@ -2792,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
@@ -2803,7 +2882,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
@@ -2814,9 +2893,9 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="26"/>
@@ -2825,7 +2904,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2838,10 +2917,10 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="15" thickTop="1"/>
-    <row r="27" spans="1:11" ht="18">
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>12</v>
@@ -2851,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
@@ -2860,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
@@ -2869,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2880,7 +2959,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
@@ -2907,7 +2986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>0</v>
       </c>
@@ -2924,7 +3003,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>0</v>
       </c>
@@ -2941,7 +3020,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>0</v>
       </c>
@@ -2958,7 +3037,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
@@ -2976,7 +3055,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
@@ -2999,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
@@ -3010,7 +3089,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
@@ -3021,9 +3100,9 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="26"/>
@@ -3032,7 +3111,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3045,8 +3124,8 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickTop="1"/>
-    <row r="44" spans="1:11" ht="23.25">
+    <row r="43" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>40</v>
       </c>
@@ -3103,20 +3182,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:K44"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3124,13 +3203,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -3148,7 +3227,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -3166,7 +3245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -3184,7 +3263,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -3202,7 +3281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3219,7 +3298,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickTop="1">
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3227,9 +3306,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>12</v>
@@ -3239,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
@@ -3248,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
@@ -3257,7 +3336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -3268,7 +3347,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -3295,7 +3374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>0</v>
       </c>
@@ -3312,7 +3391,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>0</v>
       </c>
@@ -3329,7 +3408,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>0</v>
       </c>
@@ -3346,7 +3425,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3443,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
@@ -3387,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
@@ -3398,7 +3477,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
@@ -3409,9 +3488,9 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="26"/>
@@ -3420,7 +3499,7 @@
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3433,10 +3512,10 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="15" thickTop="1"/>
-    <row r="27" spans="1:11" ht="18">
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>12</v>
@@ -3446,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
@@ -3455,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
@@ -3464,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -3475,7 +3554,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
@@ -3502,7 +3581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>0</v>
       </c>
@@ -3519,7 +3598,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>0</v>
       </c>
@@ -3536,7 +3615,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>0</v>
       </c>
@@ -3553,7 +3632,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
@@ -3571,7 +3650,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
@@ -3594,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
@@ -3605,7 +3684,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
@@ -3616,9 +3695,9 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="26"/>
@@ -3627,7 +3706,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3640,8 +3719,8 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickTop="1"/>
-    <row r="44" spans="1:11" ht="23.25">
+    <row r="43" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>40</v>
       </c>

</xml_diff>